<commit_message>
Add pins for release board
</commit_message>
<xml_diff>
--- a/docs/pins.xlsx
+++ b/docs/pins.xlsx
@@ -1,13 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19001"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22228"/>
   <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{218CA946-D8E7-406E-882E-EDF33AACE067}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="330" windowWidth="17085" windowHeight="14160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="RELEASE" sheetId="2" r:id="rId1"/>
+    <sheet name="PROTO" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -19,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="112">
   <si>
     <t>Pin#</t>
   </si>
@@ -156,9 +158,6 @@
     <t>SWD_CLK</t>
   </si>
   <si>
-    <t>Beat Sync In</t>
-  </si>
-  <si>
     <t>Off Switch In</t>
   </si>
   <si>
@@ -189,9 +188,6 @@
     <t>Gate 4 Output</t>
   </si>
   <si>
-    <t>Spare Gate Out</t>
-  </si>
-  <si>
     <t>MIDI Serial In</t>
   </si>
   <si>
@@ -213,9 +209,6 @@
     <t>Front Panel Cathode Data</t>
   </si>
   <si>
-    <t>Key Read #3</t>
-  </si>
-  <si>
     <t>Key Read #2</t>
   </si>
   <si>
@@ -258,12 +251,6 @@
     <t>A18</t>
   </si>
   <si>
-    <t>A31</t>
-  </si>
-  <si>
-    <t>A30</t>
-  </si>
-  <si>
     <t>A29</t>
   </si>
   <si>
@@ -303,9 +290,6 @@
     <t>B1</t>
   </si>
   <si>
-    <t>B0</t>
-  </si>
-  <si>
     <t>A21</t>
   </si>
   <si>
@@ -328,6 +312,51 @@
   </si>
   <si>
     <t>Beat Sync OUT</t>
+  </si>
+  <si>
+    <t>RELEASE</t>
+  </si>
+  <si>
+    <t>PROTO</t>
+  </si>
+  <si>
+    <t>B7</t>
+  </si>
+  <si>
+    <t>A12</t>
+  </si>
+  <si>
+    <t>A7</t>
+  </si>
+  <si>
+    <t>I2C0 SCL (DAC)</t>
+  </si>
+  <si>
+    <t>I2C0 SDA (DAC)</t>
+  </si>
+  <si>
+    <t>Beat Sync IN</t>
+  </si>
+  <si>
+    <t>Aux Gate Output</t>
+  </si>
+  <si>
+    <t>Aux Gate Input</t>
+  </si>
+  <si>
+    <t>I2C1 SCL (EEPROM)</t>
+  </si>
+  <si>
+    <t>I2C1 SDA (EEPROM)</t>
+  </si>
+  <si>
+    <t>A22</t>
+  </si>
+  <si>
+    <t>A23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OUT </t>
   </si>
 </sst>
 </file>
@@ -343,20 +372,25 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <strike/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color theme="4" tint="-0.249977111117893"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -371,9 +405,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -653,11 +691,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:H46"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FEAE48B6-A155-4842-8DF9-C5EF8E93AF8B}">
+  <dimension ref="B1:H46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="D45" sqref="D45"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -667,6 +705,11 @@
     <col min="5" max="5" width="4.7109375" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>97</v>
+      </c>
+    </row>
     <row r="2" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>0</v>
@@ -680,13 +723,13 @@
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="E3" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="F3" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.25">
@@ -697,24 +740,30 @@
         <v>8</v>
       </c>
       <c r="D4" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="E4" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="F4" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B5">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="2">
         <v>3</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F5" t="s">
-        <v>68</v>
+      <c r="D5" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.25">
@@ -725,7 +774,7 @@
         <v>10</v>
       </c>
       <c r="F6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.25">
@@ -768,7 +817,7 @@
         <v>15</v>
       </c>
       <c r="F11" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.25">
@@ -779,7 +828,7 @@
         <v>16</v>
       </c>
       <c r="F12" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.25">
@@ -798,41 +847,47 @@
         <v>17</v>
       </c>
       <c r="D14" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="E14" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="F14" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B15">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="15" spans="2:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="3">
         <v>13</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="F15" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B16">
+      <c r="D15" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="16" spans="2:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="3">
         <v>14</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D16" t="s">
-        <v>96</v>
-      </c>
-      <c r="E16" t="s">
-        <v>77</v>
-      </c>
-      <c r="F16" t="s">
-        <v>67</v>
+      <c r="D16" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.25">
@@ -843,47 +898,35 @@
         <v>20</v>
       </c>
       <c r="D17" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="E17" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="F17" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B18">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="3">
         <v>16</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C18" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D18" t="s">
-        <v>73</v>
-      </c>
-      <c r="E18" t="s">
-        <v>79</v>
-      </c>
-      <c r="F18" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B19">
+      <c r="F18" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="3">
         <v>17</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C19" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D19" t="s">
-        <v>73</v>
-      </c>
-      <c r="E19" t="s">
-        <v>80</v>
-      </c>
-      <c r="F19" t="s">
-        <v>64</v>
+      <c r="F19" s="3" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.25">
@@ -894,13 +937,13 @@
         <v>5</v>
       </c>
       <c r="D20" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="E20" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="F20" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.25">
@@ -911,13 +954,13 @@
         <v>21</v>
       </c>
       <c r="D21" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="E21" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="F21" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.25">
@@ -928,13 +971,13 @@
         <v>22</v>
       </c>
       <c r="D22" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="E22" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="F22" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.25">
@@ -945,13 +988,13 @@
         <v>23</v>
       </c>
       <c r="D23" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="E23" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="F23" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.25">
@@ -962,13 +1005,13 @@
         <v>24</v>
       </c>
       <c r="D24" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="E24" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="F24" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="25" spans="2:8" x14ac:dyDescent="0.25">
@@ -979,7 +1022,7 @@
         <v>25</v>
       </c>
       <c r="F25" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="26" spans="2:8" x14ac:dyDescent="0.25">
@@ -990,7 +1033,7 @@
         <v>26</v>
       </c>
       <c r="F26" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="27" spans="2:8" x14ac:dyDescent="0.25">
@@ -1000,8 +1043,14 @@
       <c r="C27" t="s">
         <v>27</v>
       </c>
+      <c r="D27" t="s">
+        <v>90</v>
+      </c>
+      <c r="E27" t="s">
+        <v>101</v>
+      </c>
       <c r="F27" t="s">
-        <v>56</v>
+        <v>105</v>
       </c>
     </row>
     <row r="28" spans="2:8" x14ac:dyDescent="0.25">
@@ -1012,16 +1061,16 @@
         <v>28</v>
       </c>
       <c r="D28" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="E28" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="F28" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H28" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
     </row>
     <row r="29" spans="2:8" x14ac:dyDescent="0.25">
@@ -1048,16 +1097,16 @@
         <v>4</v>
       </c>
       <c r="D31" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="E31" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="F31" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H31" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
     </row>
     <row r="32" spans="2:8" x14ac:dyDescent="0.25">
@@ -1068,16 +1117,16 @@
         <v>3</v>
       </c>
       <c r="D32" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="E32" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="F32" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H32" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
     </row>
     <row r="33" spans="2:8" x14ac:dyDescent="0.25">
@@ -1088,16 +1137,16 @@
         <v>2</v>
       </c>
       <c r="D33" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="E33" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="F33" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H33" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
     </row>
     <row r="34" spans="2:8" x14ac:dyDescent="0.25">
@@ -1108,7 +1157,7 @@
         <v>29</v>
       </c>
       <c r="F34" t="s">
-        <v>51</v>
+        <v>102</v>
       </c>
     </row>
     <row r="35" spans="2:8" x14ac:dyDescent="0.25">
@@ -1119,7 +1168,7 @@
         <v>30</v>
       </c>
       <c r="F35" t="s">
-        <v>50</v>
+        <v>103</v>
       </c>
     </row>
     <row r="36" spans="2:8" x14ac:dyDescent="0.25">
@@ -1130,13 +1179,13 @@
         <v>31</v>
       </c>
       <c r="D36" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="E36" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="F36" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="37" spans="2:8" x14ac:dyDescent="0.25">
@@ -1147,24 +1196,30 @@
         <v>32</v>
       </c>
       <c r="D37" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="E37" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="F37" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="38" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B38">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="38" spans="2:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B38" s="2">
         <v>36</v>
       </c>
-      <c r="C38" t="s">
+      <c r="C38" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="F38" t="s">
-        <v>48</v>
+      <c r="D38" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="E38" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="F38" s="2" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="39" spans="2:8" x14ac:dyDescent="0.25">
@@ -1174,8 +1229,14 @@
       <c r="C39" t="s">
         <v>34</v>
       </c>
+      <c r="D39" t="s">
+        <v>70</v>
+      </c>
+      <c r="E39" t="s">
+        <v>109</v>
+      </c>
       <c r="F39" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
     </row>
     <row r="40" spans="2:8" x14ac:dyDescent="0.25">
@@ -1186,44 +1247,35 @@
         <v>35</v>
       </c>
       <c r="D40" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="E40" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="F40" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="41" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B41">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="41" spans="2:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B41" s="2">
         <v>39</v>
       </c>
-      <c r="C41" t="s">
+      <c r="C41" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="D41" t="s">
-        <v>73</v>
-      </c>
-      <c r="E41" t="s">
-        <v>93</v>
-      </c>
-      <c r="F41" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="42" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B42">
+      <c r="F41" s="2" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="42" spans="2:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B42" s="2">
         <v>40</v>
       </c>
-      <c r="C42" t="s">
+      <c r="C42" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="E42" t="s">
-        <v>94</v>
-      </c>
-      <c r="F42" s="1" t="s">
-        <v>45</v>
+      <c r="F42" s="2" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="43" spans="2:8" x14ac:dyDescent="0.25">
@@ -1234,13 +1286,13 @@
         <v>38</v>
       </c>
       <c r="D43" t="s">
+        <v>90</v>
+      </c>
+      <c r="E43" t="s">
+        <v>89</v>
+      </c>
+      <c r="F43" t="s">
         <v>96</v>
-      </c>
-      <c r="E43" t="s">
-        <v>95</v>
-      </c>
-      <c r="F43" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="44" spans="2:8" x14ac:dyDescent="0.25">
@@ -1280,4 +1332,650 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="B1:J46"/>
+  <sheetViews>
+    <sheetView topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="J29" sqref="J29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="1"/>
+    <col min="2" max="2" width="5" style="1" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" style="1"/>
+    <col min="4" max="4" width="5.28515625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="4.7109375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="38.140625" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B1" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="2" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B2" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B3" s="1">
+        <v>1</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B4" s="1">
+        <v>2</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B5" s="4">
+        <v>3</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B6" s="1">
+        <v>4</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B7" s="1">
+        <v>5</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B8" s="1">
+        <v>6</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B9" s="1">
+        <v>7</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B10" s="1">
+        <v>8</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B11" s="1">
+        <v>9</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B12" s="1">
+        <v>10</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B13" s="1">
+        <v>11</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B14" s="1">
+        <v>12</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="15" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B15" s="1">
+        <v>13</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="J15" s="5"/>
+    </row>
+    <row r="16" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B16" s="1">
+        <v>14</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B17" s="1">
+        <v>15</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B18" s="1">
+        <v>16</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="J18" s="5"/>
+    </row>
+    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B19" s="1">
+        <v>17</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="J19" s="5"/>
+    </row>
+    <row r="20" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B20" s="1">
+        <v>18</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="J20" s="5"/>
+    </row>
+    <row r="21" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B21" s="1">
+        <v>19</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="22" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B22" s="1">
+        <v>20</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="23" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B23" s="1">
+        <v>21</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="24" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B24" s="1">
+        <v>22</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="25" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B25" s="1">
+        <v>23</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="26" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B26" s="1">
+        <v>24</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="27" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B27" s="1">
+        <v>25</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="28" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B28" s="1">
+        <v>26</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="H28" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="29" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B29" s="1">
+        <v>27</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="30" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B30" s="1">
+        <v>28</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="31" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B31" s="1">
+        <v>29</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="H31" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="32" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B32" s="1">
+        <v>30</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="H32" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="33" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B33" s="1">
+        <v>31</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="H33" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="34" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B34" s="1">
+        <v>32</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="35" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B35" s="1">
+        <v>33</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="36" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B36" s="1">
+        <v>34</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="37" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B37" s="1">
+        <v>35</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="38" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B38" s="4">
+        <v>36</v>
+      </c>
+      <c r="C38" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D38" s="4"/>
+      <c r="E38" s="4"/>
+      <c r="F38" s="4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="39" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B39" s="1">
+        <v>37</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F39" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="40" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B40" s="1">
+        <v>38</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="F40" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="41" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B41" s="4">
+        <v>39</v>
+      </c>
+      <c r="C41" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="D41" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="E41" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="F41" s="4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="42" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B42" s="4">
+        <v>40</v>
+      </c>
+      <c r="C42" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="D42" s="4"/>
+      <c r="E42" s="4"/>
+      <c r="F42" s="4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="43" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B43" s="1">
+        <v>41</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="F43" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="44" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B44" s="1">
+        <v>42</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F44" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="45" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B45" s="1">
+        <v>43</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F45" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="46" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B46" s="1">
+        <v>44</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F46" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
culd it be magick
</commit_message>
<xml_diff>
--- a/docs/pins.xlsx
+++ b/docs/pins.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22228"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{218CA946-D8E7-406E-882E-EDF33AACE067}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{941A81C7-9971-4684-AFD9-F0B2F6D07493}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="330" windowWidth="17085" windowHeight="14160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -694,8 +694,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FEAE48B6-A155-4842-8DF9-C5EF8E93AF8B}">
   <dimension ref="B1:H46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L14" sqref="L14"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="L18" sqref="L18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1036,21 +1036,21 @@
         <v>55</v>
       </c>
     </row>
-    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B27">
+    <row r="27" spans="2:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B27" s="2">
         <v>25</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C27" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="D27" t="s">
-        <v>90</v>
-      </c>
-      <c r="E27" t="s">
+      <c r="D27" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="E27" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="F27" t="s">
-        <v>105</v>
+      <c r="F27" s="2" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="28" spans="2:8" x14ac:dyDescent="0.25">
@@ -1109,23 +1109,23 @@
         <v>92</v>
       </c>
     </row>
-    <row r="32" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B32">
+    <row r="32" spans="2:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B32" s="2">
         <v>30</v>
       </c>
-      <c r="C32" t="s">
+      <c r="C32" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D32" t="s">
-        <v>90</v>
-      </c>
-      <c r="E32" t="s">
+      <c r="D32" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="E32" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="F32" t="s">
-        <v>52</v>
-      </c>
-      <c r="H32" t="s">
+      <c r="F32" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="H32" s="2" t="s">
         <v>93</v>
       </c>
     </row>

</xml_diff>